<commit_message>
xlsx boolean parsing fix
</commit_message>
<xml_diff>
--- a/test/artifacts/excel_different_types.xlsx
+++ b/test/artifacts/excel_different_types.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t xml:space="preserve">a</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">e</t>
   </si>
   <si>
     <t xml:space="preserve">goh, idd</t>
@@ -46,11 +49,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
-    <numFmt numFmtId="166" formatCode="D/MM/YY\ H:MM;@"/>
-    <numFmt numFmtId="167" formatCode="D/M/YYYY\ H:MM"/>
+    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="167" formatCode="D/MM/YY\ H:MM;@"/>
+    <numFmt numFmtId="168" formatCode="D/M/YYYY\ H:MM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -117,7 +121,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -126,15 +130,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,19 +163,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.5459183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.83673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.83673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,8 +192,11 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>40961</v>
       </c>
@@ -197,20 +209,28 @@
       <c r="D2" s="0" t="n">
         <v>42000.22323</v>
       </c>
+      <c r="E2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>222</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>42000.22323</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -221,16 +241,20 @@
         <v>42000</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -245,18 +269,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.84"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -271,18 +295,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.83673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.84"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>